<commit_message>
Added credit score adjustment rate generator. Added several helper methods to simplify logic for the remainder of the adjustment rate generators.
</commit_message>
<xml_diff>
--- a/CSA Table.xlsx
+++ b/CSA Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\source\repos\Sprout Mortgage Prog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03B94CE2-9491-4F18-BF32-E32ACA1D71C8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628A9A26-778A-4BEC-AC9B-86C7DE23F0B3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{3B0B612E-D7FF-44E7-B09D-6EF79A13A117}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B0B612E-D7FF-44E7-B09D-6EF79A13A117}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -238,6 +238,25 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -253,6 +272,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -262,28 +284,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,348 +601,348 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="3"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="10"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="3"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="8"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="16"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="4">
         <v>-0.25</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="4">
         <v>-0.25</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="4">
         <v>-0.25</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="4">
         <v>-0.125</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="4">
         <v>0</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="4">
         <v>0</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="4">
         <v>0.125</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="4">
         <v>0.25</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="4">
         <v>0.625</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="4">
         <v>-0.125</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="4">
         <v>-0.125</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="4">
         <v>-0.125</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="4">
         <v>0</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="4">
         <v>0.125</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="4">
         <v>0.25</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="4">
         <v>0.25</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="4">
         <v>0.375</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="4">
         <v>0.75</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="4">
         <v>0</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="4">
         <v>0.05</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="4">
         <v>0.05</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="4">
         <v>0.17499999999999999</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="4">
         <v>0.3</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="4">
         <v>0.3</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="4">
         <v>0.42499999999999999</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="4">
         <v>0.5</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="4">
         <v>0.875</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="4">
         <v>0.125</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="4">
         <v>0.17499999999999999</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="4">
         <v>0.17499999999999999</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="4">
         <v>0.3</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="4">
         <v>0.3</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="4">
         <v>0.42499999999999999</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="4">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="4">
         <v>0.75</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="4">
         <v>1.25</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="4">
         <v>0.25</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="4">
         <v>0.3</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="4">
         <v>0.3</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="4">
         <v>0.42499999999999999</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="4">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="4">
         <v>0.67500000000000004</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="4">
         <v>0.8</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="4">
         <v>1.25</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="4">
         <v>0.375</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="4">
         <v>0.42499999999999999</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="4">
         <v>0.42499999999999999</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="4">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="4">
         <v>0.67500000000000004</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="4">
         <v>0.92500000000000004</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="4">
         <v>1.175</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="4">
         <v>1.625</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="4">
         <v>0.5</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="4">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="4">
         <v>0.55000000000000004</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="4">
         <v>0.67500000000000004</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="4">
         <v>0.92500000000000004</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="4">
         <v>1.3</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="4">
         <v>1.8</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="4">
         <v>2.125</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="4">
         <v>0.625</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="4">
         <v>0.67500000000000004</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="4">
         <v>0.67500000000000004</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="4">
         <v>0.8</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>